<commit_message>
v0.16: HexagonalSquares are drawn on maze image.
</commit_message>
<xml_diff>
--- a/rsc/mazes/hexagon/hmz_takochan.xlsx
+++ b/rsc/mazes/hexagon/hmz_takochan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="squares" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,13 +27,13 @@
     <t xml:space="preserve">_</t>
   </si>
   <si>
-    <t xml:space="preserve">F</t>
+    <t xml:space="preserve">T</t>
   </si>
   <si>
     <t xml:space="preserve">S</t>
   </si>
   <si>
-    <t xml:space="preserve">G</t>
+    <t xml:space="preserve">B</t>
   </si>
   <si>
     <t xml:space="preserve">ice</t>
@@ -165,11 +165,11 @@
   </sheetPr>
   <dimension ref="B2:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.59765625" defaultRowHeight="50.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.60546875" defaultRowHeight="50.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="9.59"/>
   </cols>
@@ -187,7 +187,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
@@ -211,11 +211,11 @@
   </sheetPr>
   <dimension ref="B2:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.59765625" defaultRowHeight="50.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.60546875" defaultRowHeight="50.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="9.59"/>
   </cols>
@@ -236,7 +236,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -261,7 +261,7 @@
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.59765625" defaultRowHeight="50.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.60546875" defaultRowHeight="50.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="2" width="9.59"/>
   </cols>

</xml_diff>

<commit_message>
v0.16: Fix borders drawing : first border is UP border. Border thickness is taken into account when computing maze image dimensions.
</commit_message>
<xml_diff>
--- a/rsc/mazes/hexagon/hmz_takochan.xlsx
+++ b/rsc/mazes/hexagon/hmz_takochan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="squares" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t xml:space="preserve">_</t>
   </si>
@@ -39,16 +39,20 @@
     <t xml:space="preserve">ice</t>
   </si>
   <si>
-    <t xml:space="preserve">W
-_ _
-_ _
-W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_
-W W
-W _
-_</t>
+    <t xml:space="preserve">W _ _
+W W _</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W _ _
+W _ _</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ W _
+W W _</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ W _
+_ W W</t>
   </si>
 </sst>
 </file>
@@ -211,7 +215,7 @@
   </sheetPr>
   <dimension ref="B2:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -255,10 +259,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:D3"/>
+  <dimension ref="B2:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.60546875" defaultRowHeight="50.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -271,17 +275,18 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>